<commit_message>
household energy use data
</commit_message>
<xml_diff>
--- a/chapters/ch07-Households/datasets/Household_energy_use_data.xlsx
+++ b/chapters/ch07-Households/datasets/Household_energy_use_data.xlsx
@@ -5,27 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/MCBook2021/chapters/ch07-Households/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch07-Households/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4FA0F6-CB68-D84F-A70F-DCDA27E262A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA9F645-F700-A947-ADFE-354383E0B0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28840" yWindow="2720" windowWidth="20200" windowHeight="18340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28840" yWindow="2720" windowWidth="20200" windowHeight="18340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="9" r:id="rId1"/>
     <sheet name="Figure 1. Trends in Consumption" sheetId="7" r:id="rId2"/>
     <sheet name="Figure 2. Avg State Cons andExp" sheetId="4" r:id="rId3"/>
     <sheet name="us-average-by-census-region-sel" sheetId="8" r:id="rId4"/>
+    <sheet name="data" sheetId="10" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">data!$2:$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -120,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="172">
   <si>
     <t>Total U.S.</t>
   </si>
@@ -255,6 +257,715 @@
   </si>
   <si>
     <t>Data from: https://www.eia.gov/energyexplained/use-of-energy/homes.php</t>
+  </si>
+  <si>
+    <t>Energy [10^6 BTU/household]</t>
+  </si>
+  <si>
+    <t>Housing units [10^6]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Housing characteristics data were collected between August 2015 and April 2016.
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Total U.S. includes all primary occupied housing units in the 50 states and the District of Columbia. Vacant housing units, seasonal units, second homes, military houses, and group quarters are excluded.
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Total square footage includes all basements, finished or conditioned (heated or cooled) areas of attics, and conditioned garage space that is attached to the home. Unconditioned and unfinished areas in attics and attached garages are excluded. The square footage for some housing units was calculated based on measurements taken by the interviewer. For households responding without the presence of an interviewer, square footage was imputed based on characteristics of the housing unit. See 2015 RECS Square Footage Methodology for full details about data collection and processing.
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">When calculating average heated and cooled square footage all housing units are considered, including those that are not heated or cooled.
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Housing units are classified using criteria created by the U.S. Census Bureau based on 2010 Census data. Urbanized areas are densely settled groupings of blocks or tracts with 50,000 or more people, while urban clusters have at least 2,500 but less than 50,000 people. All other areas are rural.
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>These climate regions were created by the Building America program, sponsored by the U.S. Department of Energy’s Office of Energy Efficiency and Renewable Energy (EERE).</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Households that use propane only for outdoor grilling are excluded from the RECS estimate of households using propane.          
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rented includes households that occupy their primary housing units without paying rent.
+     Notes:  Because of rounding, data may not sum to totals.  See RECS Terminology for definition of terms used in these tables.
+     Source: U.S. Energy Information Administration, Office of Energy Consumption and Efficiency Statistics, Forms EIA-457A and EIA-457C of the 2015 Residential Energy Consumption Survey.</t>
+    </r>
+  </si>
+  <si>
+    <t>Rented</t>
+  </si>
+  <si>
+    <t>Owned</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <r>
+      <t>Ownership of housing unit</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+  </si>
+  <si>
+    <t>$140,000 or more</t>
+  </si>
+  <si>
+    <t>$120,000 to $139,999</t>
+  </si>
+  <si>
+    <t>$100,000 to $119,999</t>
+  </si>
+  <si>
+    <t>$80,000 to $99,999</t>
+  </si>
+  <si>
+    <t>$60,000 to $79,999</t>
+  </si>
+  <si>
+    <t>$40,000 to $59,999</t>
+  </si>
+  <si>
+    <t>$20,000 to $39,999</t>
+  </si>
+  <si>
+    <t>Less than $20,000</t>
+  </si>
+  <si>
+    <t>2015 annual household income</t>
+  </si>
+  <si>
+    <t>6 or more members</t>
+  </si>
+  <si>
+    <t>5 members</t>
+  </si>
+  <si>
+    <t>4 members</t>
+  </si>
+  <si>
+    <t>3 members</t>
+  </si>
+  <si>
+    <t>2 members</t>
+  </si>
+  <si>
+    <t>1 member</t>
+  </si>
+  <si>
+    <t>Number of household members</t>
+  </si>
+  <si>
+    <t>Triple-pane glass</t>
+  </si>
+  <si>
+    <t>Double-pane glass</t>
+  </si>
+  <si>
+    <t>Single-pane glass</t>
+  </si>
+  <si>
+    <t>Type of glass in windows</t>
+  </si>
+  <si>
+    <t>No insulation</t>
+  </si>
+  <si>
+    <t>Poorly insulated</t>
+  </si>
+  <si>
+    <t>Adequately insulated</t>
+  </si>
+  <si>
+    <t>Well insulated</t>
+  </si>
+  <si>
+    <t>Adequacy of insulation</t>
+  </si>
+  <si>
+    <t>Not asked (apartments and mobile homes)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Unfinished basement</t>
+  </si>
+  <si>
+    <t>Finished basement</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Have a basement</t>
+  </si>
+  <si>
+    <t>5 or more</t>
+  </si>
+  <si>
+    <t>Number of bedrooms</t>
+  </si>
+  <si>
+    <t>9 or more</t>
+  </si>
+  <si>
+    <t>1 or 2</t>
+  </si>
+  <si>
+    <t>Total number of rooms (excluding bathrooms)</t>
+  </si>
+  <si>
+    <t>80 or more</t>
+  </si>
+  <si>
+    <t>60 to 79</t>
+  </si>
+  <si>
+    <t>40 to 59</t>
+  </si>
+  <si>
+    <t>20 to 39</t>
+  </si>
+  <si>
+    <t>Fewer than 20</t>
+  </si>
+  <si>
+    <t>Indoor light bulbs installed</t>
+  </si>
+  <si>
+    <t>Some other fuel</t>
+  </si>
+  <si>
+    <t>Fuel oil/kerosene</t>
+  </si>
+  <si>
+    <t>Propane</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Natural gas</t>
+  </si>
+  <si>
+    <t>Fuel used by main water heater</t>
+  </si>
+  <si>
+    <t>Do not use air-conditioning equipment</t>
+  </si>
+  <si>
+    <t>Use individual air-conditioning units</t>
+  </si>
+  <si>
+    <t>Use central air-conditioning equipment</t>
+  </si>
+  <si>
+    <t>Type of air-conditioning equipment used (more than one may apply)</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Do not use heating equipment</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Main space heating fuel</t>
+  </si>
+  <si>
+    <t>Not asked (apartments)</t>
+  </si>
+  <si>
+    <t>Distributed solar generation</t>
+  </si>
+  <si>
+    <r>
+      <t>Propane</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <t>Fuels used for any use (more than one may apply)</t>
+  </si>
+  <si>
+    <t>Split level</t>
+  </si>
+  <si>
+    <t>Three or more stories</t>
+  </si>
+  <si>
+    <t>Two stories</t>
+  </si>
+  <si>
+    <t>One story</t>
+  </si>
+  <si>
+    <t>Number of stories</t>
+  </si>
+  <si>
+    <t>2010 to 2015</t>
+  </si>
+  <si>
+    <t>2000 to 2009</t>
+  </si>
+  <si>
+    <t>1990 to 1999</t>
+  </si>
+  <si>
+    <t>1980 to 1989</t>
+  </si>
+  <si>
+    <t>1970 to 1979</t>
+  </si>
+  <si>
+    <t>1960 to 1969</t>
+  </si>
+  <si>
+    <t>1950 to 1959</t>
+  </si>
+  <si>
+    <t>Before 1950</t>
+  </si>
+  <si>
+    <t>Year of construction</t>
+  </si>
+  <si>
+    <t>Mobile homes</t>
+  </si>
+  <si>
+    <t>Apartments in buildings with 5 or more units</t>
+  </si>
+  <si>
+    <t>Apartments in buildings with 2-4 units</t>
+  </si>
+  <si>
+    <t>Single-family attached</t>
+  </si>
+  <si>
+    <t>Single-family detached</t>
+  </si>
+  <si>
+    <t>Housing unit type</t>
+  </si>
+  <si>
+    <t>Marine</t>
+  </si>
+  <si>
+    <t>Hot-humid</t>
+  </si>
+  <si>
+    <t>Mixed-dry/Hot-dry</t>
+  </si>
+  <si>
+    <t>Mixed-humid</t>
+  </si>
+  <si>
+    <t>Very cold/Cold</t>
+  </si>
+  <si>
+    <r>
+      <t>Climate region</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <t>Not in metropolitan or micropolitan statistical area</t>
+  </si>
+  <si>
+    <t>In micropolitan statistical area</t>
+  </si>
+  <si>
+    <t>In metropolitan statistical area</t>
+  </si>
+  <si>
+    <t>Metropolitan or micropolitan statistical area</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>Urban cluster</t>
+  </si>
+  <si>
+    <t>Urbanized area</t>
+  </si>
+  <si>
+    <t>Urban</t>
+  </si>
+  <si>
+    <r>
+      <t>Census urban/rural classification</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <t>Pacific</t>
+  </si>
+  <si>
+    <t>Mountain South</t>
+  </si>
+  <si>
+    <t>Mountain North</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>West South Central</t>
+  </si>
+  <si>
+    <t>East South Central</t>
+  </si>
+  <si>
+    <t>South Atlantic</t>
+  </si>
+  <si>
+    <t>West North Central</t>
+  </si>
+  <si>
+    <t>East North Central</t>
+  </si>
+  <si>
+    <t>Middle Atlantic</t>
+  </si>
+  <si>
+    <t>New England</t>
+  </si>
+  <si>
+    <t>Census region and division</t>
+  </si>
+  <si>
+    <t>All homes</t>
+  </si>
+  <si>
+    <t>Cooled</t>
+  </si>
+  <si>
+    <t>Heated</t>
+  </si>
+  <si>
+    <r>
+      <t>Total</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cooled</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Heated</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Total U.S.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Average square footage 
+per household member</t>
+  </si>
+  <si>
+    <t>Average square footage 
+per housing unit</t>
+  </si>
+  <si>
+    <t>Number of housing units (million)</t>
+  </si>
+  <si>
+    <r>
+      <t>Table HC10.9  Average square footage of U.S. homes, 2015</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>Release date: October 2017
+Revised date: May 2018</t>
+  </si>
+  <si>
+    <t>data from: https://www.eia.gov/consumption/residential/data/2015/#squarefootage</t>
   </si>
 </sst>
 </file>
@@ -265,7 +976,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="@*."/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +1015,85 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -313,7 +1103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -321,12 +1111,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFont="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
@@ -341,10 +1220,88 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="4" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="5" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="8">
+    <cellStyle name="Body: normal cell" xfId="3" xr:uid="{5F7BF65E-24C2-C540-AFAB-611601D034F7}"/>
+    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{D83CCA24-64DE-C149-B858-D1C43977C9F8}"/>
+    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{1F2E4016-1ADE-4046-AC6A-B429AEB86BB4}"/>
+    <cellStyle name="Header: top rows" xfId="6" xr:uid="{62221018-836C-0744-9203-4ED3A570572F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{4993F3BE-82B3-E44C-B48F-7E898CFB4071}"/>
+    <cellStyle name="Parent row" xfId="4" xr:uid="{5D1B63A1-57DA-9349-87C3-E8DEA93A8D51}"/>
+    <cellStyle name="Table title" xfId="7" xr:uid="{377025B3-17E8-C842-A69D-64B003043AA2}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4548,7 +5505,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4557,13 +5514,11 @@
       <c r="A1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="str">
-        <f>'Figure 1. Trends in Consumption'!B2</f>
-        <v>Average Consumption (million btu per household)</v>
-      </c>
-      <c r="C1" t="str">
-        <f>'Figure 1. Trends in Consumption'!D2</f>
-        <v>Number Housing Units</v>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4828,6 +5783,10 @@
       <c r="B37">
         <f>'us-average-by-census-region-sel'!E7</f>
         <v>77.099999999999994</v>
+      </c>
+      <c r="C37">
+        <f>data!B5</f>
+        <v>118.2</v>
       </c>
     </row>
   </sheetData>
@@ -4840,8 +5799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5028,7 +5987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
@@ -5546,4 +6505,3661 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F9B757-12BF-CF44-BC1A-B01442B5ACE3}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J142"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K142" sqref="K142"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="8" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="J2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+      <c r="B3" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="23">
+        <v>118.2</v>
+      </c>
+      <c r="C5" s="22">
+        <v>2008</v>
+      </c>
+      <c r="D5" s="22">
+        <v>1754</v>
+      </c>
+      <c r="E5" s="22">
+        <v>1375</v>
+      </c>
+      <c r="F5" s="22">
+        <v>789</v>
+      </c>
+      <c r="G5" s="22">
+        <v>689</v>
+      </c>
+      <c r="H5" s="22">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="12">
+        <v>21</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2090</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1791</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1015</v>
+      </c>
+      <c r="F7" s="11">
+        <v>843</v>
+      </c>
+      <c r="G7" s="11">
+        <v>722</v>
+      </c>
+      <c r="H7" s="11">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="C8" s="11">
+        <v>2186</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1861</v>
+      </c>
+      <c r="E8" s="11">
+        <v>783</v>
+      </c>
+      <c r="F8" s="11">
+        <v>906</v>
+      </c>
+      <c r="G8" s="11">
+        <v>771</v>
+      </c>
+      <c r="H8" s="11">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="12">
+        <v>15.4</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2055</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1765</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1100</v>
+      </c>
+      <c r="F9" s="11">
+        <v>820</v>
+      </c>
+      <c r="G9" s="11">
+        <v>704</v>
+      </c>
+      <c r="H9" s="11">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="12">
+        <v>26.4</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2278</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2043</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1624</v>
+      </c>
+      <c r="F10" s="11">
+        <v>913</v>
+      </c>
+      <c r="G10" s="11">
+        <v>819</v>
+      </c>
+      <c r="H10" s="11">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="12">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="C11" s="11">
+        <v>2250</v>
+      </c>
+      <c r="D11" s="11">
+        <v>2051</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1563</v>
+      </c>
+      <c r="F11" s="11">
+        <v>885</v>
+      </c>
+      <c r="G11" s="11">
+        <v>806</v>
+      </c>
+      <c r="H11" s="11">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="12">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2338</v>
+      </c>
+      <c r="D12" s="11">
+        <v>2024</v>
+      </c>
+      <c r="E12" s="11">
+        <v>1758</v>
+      </c>
+      <c r="F12" s="11">
+        <v>981</v>
+      </c>
+      <c r="G12" s="11">
+        <v>849</v>
+      </c>
+      <c r="H12" s="11">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="12">
+        <v>44.4</v>
+      </c>
+      <c r="C13" s="11">
+        <v>1939</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1679</v>
+      </c>
+      <c r="E13" s="11">
+        <v>1572</v>
+      </c>
+      <c r="F13" s="11">
+        <v>767</v>
+      </c>
+      <c r="G13" s="11">
+        <v>665</v>
+      </c>
+      <c r="H13" s="11">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="12">
+        <v>23.5</v>
+      </c>
+      <c r="C14" s="11">
+        <v>1999</v>
+      </c>
+      <c r="D14" s="11">
+        <v>1669</v>
+      </c>
+      <c r="E14" s="11">
+        <v>1615</v>
+      </c>
+      <c r="F14" s="11">
+        <v>801</v>
+      </c>
+      <c r="G14" s="11">
+        <v>669</v>
+      </c>
+      <c r="H14" s="11">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="12">
+        <v>7.2</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1870</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1625</v>
+      </c>
+      <c r="E15" s="11">
+        <v>1393</v>
+      </c>
+      <c r="F15" s="11">
+        <v>743</v>
+      </c>
+      <c r="G15" s="11">
+        <v>645</v>
+      </c>
+      <c r="H15" s="11">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="12">
+        <v>13.8</v>
+      </c>
+      <c r="C16" s="11">
+        <v>1873</v>
+      </c>
+      <c r="D16" s="11">
+        <v>1725</v>
+      </c>
+      <c r="E16" s="11">
+        <v>1592</v>
+      </c>
+      <c r="F16" s="11">
+        <v>724</v>
+      </c>
+      <c r="G16" s="11">
+        <v>667</v>
+      </c>
+      <c r="H16" s="11">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="12">
+        <v>26.4</v>
+      </c>
+      <c r="C17" s="11">
+        <v>1791</v>
+      </c>
+      <c r="D17" s="11">
+        <v>1563</v>
+      </c>
+      <c r="E17" s="11">
+        <v>1081</v>
+      </c>
+      <c r="F17" s="11">
+        <v>667</v>
+      </c>
+      <c r="G17" s="11">
+        <v>582</v>
+      </c>
+      <c r="H17" s="11">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="12">
+        <v>8.5</v>
+      </c>
+      <c r="C18" s="11">
+        <v>2007</v>
+      </c>
+      <c r="D18" s="11">
+        <v>1896</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1360</v>
+      </c>
+      <c r="F18" s="11">
+        <v>777</v>
+      </c>
+      <c r="G18" s="11">
+        <v>734</v>
+      </c>
+      <c r="H18" s="11">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="C19" s="11">
+        <v>2171</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2037</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1294</v>
+      </c>
+      <c r="F19" s="11">
+        <v>812</v>
+      </c>
+      <c r="G19" s="11">
+        <v>761</v>
+      </c>
+      <c r="H19" s="11">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="12">
+        <v>4.3</v>
+      </c>
+      <c r="C20" s="11">
+        <v>1844</v>
+      </c>
+      <c r="D20" s="11">
+        <v>1755</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1427</v>
+      </c>
+      <c r="F20" s="11">
+        <v>741</v>
+      </c>
+      <c r="G20" s="11">
+        <v>705</v>
+      </c>
+      <c r="H20" s="11">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="12">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1689</v>
+      </c>
+      <c r="D21" s="11">
+        <v>1405</v>
+      </c>
+      <c r="E21" s="11">
+        <v>947</v>
+      </c>
+      <c r="F21" s="11">
+        <v>617</v>
+      </c>
+      <c r="G21" s="11">
+        <v>513</v>
+      </c>
+      <c r="H21" s="11">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" s="12">
+        <v>94.7</v>
+      </c>
+      <c r="C23" s="11">
+        <v>1931</v>
+      </c>
+      <c r="D23" s="11">
+        <v>1684</v>
+      </c>
+      <c r="E23" s="11">
+        <v>1359</v>
+      </c>
+      <c r="F23" s="11">
+        <v>762</v>
+      </c>
+      <c r="G23" s="11">
+        <v>665</v>
+      </c>
+      <c r="H23" s="11">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" s="12">
+        <v>82.2</v>
+      </c>
+      <c r="C24" s="11">
+        <v>1942</v>
+      </c>
+      <c r="D24" s="11">
+        <v>1690</v>
+      </c>
+      <c r="E24" s="11">
+        <v>1374</v>
+      </c>
+      <c r="F24" s="11">
+        <v>760</v>
+      </c>
+      <c r="G24" s="11">
+        <v>662</v>
+      </c>
+      <c r="H24" s="11">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="12">
+        <v>12.5</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1861</v>
+      </c>
+      <c r="D25" s="11">
+        <v>1646</v>
+      </c>
+      <c r="E25" s="11">
+        <v>1259</v>
+      </c>
+      <c r="F25" s="11">
+        <v>777</v>
+      </c>
+      <c r="G25" s="11">
+        <v>687</v>
+      </c>
+      <c r="H25" s="11">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" s="12">
+        <v>23.5</v>
+      </c>
+      <c r="C26" s="11">
+        <v>2320</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2039</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1439</v>
+      </c>
+      <c r="F26" s="11">
+        <v>891</v>
+      </c>
+      <c r="G26" s="11">
+        <v>783</v>
+      </c>
+      <c r="H26" s="11">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="12">
+        <v>98.5</v>
+      </c>
+      <c r="C28" s="11">
+        <v>2014</v>
+      </c>
+      <c r="D28" s="11">
+        <v>1753</v>
+      </c>
+      <c r="E28" s="11">
+        <v>1403</v>
+      </c>
+      <c r="F28" s="11">
+        <v>785</v>
+      </c>
+      <c r="G28" s="11">
+        <v>683</v>
+      </c>
+      <c r="H28" s="11">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="12">
+        <v>12.3</v>
+      </c>
+      <c r="C29" s="11">
+        <v>2014</v>
+      </c>
+      <c r="D29" s="11">
+        <v>1784</v>
+      </c>
+      <c r="E29" s="11">
+        <v>1299</v>
+      </c>
+      <c r="F29" s="11">
+        <v>830</v>
+      </c>
+      <c r="G29" s="11">
+        <v>735</v>
+      </c>
+      <c r="H29" s="11">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="12">
+        <v>7.4</v>
+      </c>
+      <c r="C30" s="11">
+        <v>1930</v>
+      </c>
+      <c r="D30" s="11">
+        <v>1726</v>
+      </c>
+      <c r="E30" s="11">
+        <v>1130</v>
+      </c>
+      <c r="F30" s="11">
+        <v>775</v>
+      </c>
+      <c r="G30" s="11">
+        <v>693</v>
+      </c>
+      <c r="H30" s="11">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="12">
+        <v>42.5</v>
+      </c>
+      <c r="C32" s="11">
+        <v>2228</v>
+      </c>
+      <c r="D32" s="11">
+        <v>2007</v>
+      </c>
+      <c r="E32" s="11">
+        <v>1334</v>
+      </c>
+      <c r="F32" s="11">
+        <v>894</v>
+      </c>
+      <c r="G32" s="11">
+        <v>805</v>
+      </c>
+      <c r="H32" s="11">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="12">
+        <v>33.5</v>
+      </c>
+      <c r="C33" s="11">
+        <v>2073</v>
+      </c>
+      <c r="D33" s="11">
+        <v>1771</v>
+      </c>
+      <c r="E33" s="11">
+        <v>1530</v>
+      </c>
+      <c r="F33" s="11">
+        <v>807</v>
+      </c>
+      <c r="G33" s="11">
+        <v>689</v>
+      </c>
+      <c r="H33" s="11">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" s="12">
+        <v>12.7</v>
+      </c>
+      <c r="C34" s="11">
+        <v>1668</v>
+      </c>
+      <c r="D34" s="11">
+        <v>1416</v>
+      </c>
+      <c r="E34" s="11">
+        <v>1256</v>
+      </c>
+      <c r="F34" s="11">
+        <v>620</v>
+      </c>
+      <c r="G34" s="11">
+        <v>526</v>
+      </c>
+      <c r="H34" s="11">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B35" s="12">
+        <v>22.8</v>
+      </c>
+      <c r="C35" s="11">
+        <v>1742</v>
+      </c>
+      <c r="D35" s="11">
+        <v>1495</v>
+      </c>
+      <c r="E35" s="11">
+        <v>1483</v>
+      </c>
+      <c r="F35" s="11">
+        <v>704</v>
+      </c>
+      <c r="G35" s="11">
+        <v>604</v>
+      </c>
+      <c r="H35" s="11">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="12">
+        <v>6.7</v>
+      </c>
+      <c r="C36" s="11">
+        <v>1842</v>
+      </c>
+      <c r="D36" s="11">
+        <v>1598</v>
+      </c>
+      <c r="E36" s="11">
+        <v>713</v>
+      </c>
+      <c r="F36" s="11">
+        <v>667</v>
+      </c>
+      <c r="G36" s="11">
+        <v>579</v>
+      </c>
+      <c r="H36" s="11">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="12">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="C38" s="11">
+        <v>2553</v>
+      </c>
+      <c r="D38" s="11">
+        <v>2210</v>
+      </c>
+      <c r="E38" s="11">
+        <v>1757</v>
+      </c>
+      <c r="F38" s="11">
+        <v>934</v>
+      </c>
+      <c r="G38" s="11">
+        <v>809</v>
+      </c>
+      <c r="H38" s="11">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="12">
+        <v>7</v>
+      </c>
+      <c r="C39" s="11">
+        <v>1774</v>
+      </c>
+      <c r="D39" s="11">
+        <v>1528</v>
+      </c>
+      <c r="E39" s="11">
+        <v>1186</v>
+      </c>
+      <c r="F39" s="11">
+        <v>725</v>
+      </c>
+      <c r="G39" s="11">
+        <v>624</v>
+      </c>
+      <c r="H39" s="11">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="12">
+        <v>9.4</v>
+      </c>
+      <c r="C40" s="11">
+        <v>1020</v>
+      </c>
+      <c r="D40" s="11">
+        <v>969</v>
+      </c>
+      <c r="E40" s="11">
+        <v>603</v>
+      </c>
+      <c r="F40" s="11">
+        <v>426</v>
+      </c>
+      <c r="G40" s="11">
+        <v>404</v>
+      </c>
+      <c r="H40" s="11">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="12">
+        <v>21.1</v>
+      </c>
+      <c r="C41" s="11">
+        <v>882</v>
+      </c>
+      <c r="D41" s="11">
+        <v>782</v>
+      </c>
+      <c r="E41" s="11">
+        <v>627</v>
+      </c>
+      <c r="F41" s="11">
+        <v>447</v>
+      </c>
+      <c r="G41" s="11">
+        <v>396</v>
+      </c>
+      <c r="H41" s="11">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="C42" s="11">
+        <v>1198</v>
+      </c>
+      <c r="D42" s="11">
+        <v>1145</v>
+      </c>
+      <c r="E42" s="11">
+        <v>813</v>
+      </c>
+      <c r="F42" s="11">
+        <v>456</v>
+      </c>
+      <c r="G42" s="11">
+        <v>436</v>
+      </c>
+      <c r="H42" s="11">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="12">
+        <v>20.8</v>
+      </c>
+      <c r="C44" s="11">
+        <v>2012</v>
+      </c>
+      <c r="D44" s="11">
+        <v>1675</v>
+      </c>
+      <c r="E44" s="11">
+        <v>935</v>
+      </c>
+      <c r="F44" s="11">
+        <v>806</v>
+      </c>
+      <c r="G44" s="11">
+        <v>671</v>
+      </c>
+      <c r="H44" s="11">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="12">
+        <v>12.6</v>
+      </c>
+      <c r="C45" s="11">
+        <v>1867</v>
+      </c>
+      <c r="D45" s="11">
+        <v>1607</v>
+      </c>
+      <c r="E45" s="11">
+        <v>1111</v>
+      </c>
+      <c r="F45" s="11">
+        <v>763</v>
+      </c>
+      <c r="G45" s="11">
+        <v>657</v>
+      </c>
+      <c r="H45" s="11">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="12">
+        <v>12.8</v>
+      </c>
+      <c r="C46" s="11">
+        <v>1874</v>
+      </c>
+      <c r="D46" s="11">
+        <v>1622</v>
+      </c>
+      <c r="E46" s="11">
+        <v>1197</v>
+      </c>
+      <c r="F46" s="11">
+        <v>801</v>
+      </c>
+      <c r="G46" s="11">
+        <v>693</v>
+      </c>
+      <c r="H46" s="11">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" s="12">
+        <v>18.3</v>
+      </c>
+      <c r="C47" s="11">
+        <v>1767</v>
+      </c>
+      <c r="D47" s="11">
+        <v>1559</v>
+      </c>
+      <c r="E47" s="11">
+        <v>1243</v>
+      </c>
+      <c r="F47" s="11">
+        <v>701</v>
+      </c>
+      <c r="G47" s="11">
+        <v>618</v>
+      </c>
+      <c r="H47" s="11">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="12">
+        <v>16</v>
+      </c>
+      <c r="C48" s="11">
+        <v>1831</v>
+      </c>
+      <c r="D48" s="11">
+        <v>1608</v>
+      </c>
+      <c r="E48" s="11">
+        <v>1350</v>
+      </c>
+      <c r="F48" s="11">
+        <v>760</v>
+      </c>
+      <c r="G48" s="11">
+        <v>667</v>
+      </c>
+      <c r="H48" s="11">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="12">
+        <v>16.8</v>
+      </c>
+      <c r="C49" s="11">
+        <v>2185</v>
+      </c>
+      <c r="D49" s="11">
+        <v>1960</v>
+      </c>
+      <c r="E49" s="11">
+        <v>1704</v>
+      </c>
+      <c r="F49" s="11">
+        <v>811</v>
+      </c>
+      <c r="G49" s="11">
+        <v>728</v>
+      </c>
+      <c r="H49" s="11">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" s="12">
+        <v>17</v>
+      </c>
+      <c r="C50" s="11">
+        <v>2388</v>
+      </c>
+      <c r="D50" s="11">
+        <v>2132</v>
+      </c>
+      <c r="E50" s="11">
+        <v>1954</v>
+      </c>
+      <c r="F50" s="11">
+        <v>855</v>
+      </c>
+      <c r="G50" s="11">
+        <v>763</v>
+      </c>
+      <c r="H50" s="11">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="12">
+        <v>3.8</v>
+      </c>
+      <c r="C51" s="11">
+        <v>2347</v>
+      </c>
+      <c r="D51" s="11">
+        <v>2081</v>
+      </c>
+      <c r="E51" s="11">
+        <v>1944</v>
+      </c>
+      <c r="F51" s="11">
+        <v>837</v>
+      </c>
+      <c r="G51" s="11">
+        <v>742</v>
+      </c>
+      <c r="H51" s="11">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" s="12">
+        <v>47.5</v>
+      </c>
+      <c r="C53" s="11">
+        <v>2054</v>
+      </c>
+      <c r="D53" s="11">
+        <v>1755</v>
+      </c>
+      <c r="E53" s="11">
+        <v>1421</v>
+      </c>
+      <c r="F53" s="11">
+        <v>808</v>
+      </c>
+      <c r="G53" s="11">
+        <v>690</v>
+      </c>
+      <c r="H53" s="11">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" s="12">
+        <v>29.5</v>
+      </c>
+      <c r="C54" s="11">
+        <v>3131</v>
+      </c>
+      <c r="D54" s="11">
+        <v>2732</v>
+      </c>
+      <c r="E54" s="11">
+        <v>2149</v>
+      </c>
+      <c r="F54" s="11">
+        <v>1057</v>
+      </c>
+      <c r="G54" s="11">
+        <v>922</v>
+      </c>
+      <c r="H54" s="11">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="C55" s="11">
+        <v>2945</v>
+      </c>
+      <c r="D55" s="11">
+        <v>2585</v>
+      </c>
+      <c r="E55" s="11">
+        <v>1601</v>
+      </c>
+      <c r="F55" s="11">
+        <v>1090</v>
+      </c>
+      <c r="G55" s="11">
+        <v>957</v>
+      </c>
+      <c r="H55" s="11">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="12">
+        <v>2.1</v>
+      </c>
+      <c r="C56" s="11">
+        <v>2828</v>
+      </c>
+      <c r="D56" s="11">
+        <v>2589</v>
+      </c>
+      <c r="E56" s="11">
+        <v>2065</v>
+      </c>
+      <c r="F56" s="11">
+        <v>990</v>
+      </c>
+      <c r="G56" s="11">
+        <v>907</v>
+      </c>
+      <c r="H56" s="11">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="12">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="C57" s="11">
+        <v>974</v>
+      </c>
+      <c r="D57" s="11">
+        <v>895</v>
+      </c>
+      <c r="E57" s="11">
+        <v>655</v>
+      </c>
+      <c r="F57" s="11">
+        <v>443</v>
+      </c>
+      <c r="G57" s="11">
+        <v>407</v>
+      </c>
+      <c r="H57" s="11">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H58" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="12">
+        <v>118.2</v>
+      </c>
+      <c r="C59" s="11">
+        <v>2008</v>
+      </c>
+      <c r="D59" s="11">
+        <v>1754</v>
+      </c>
+      <c r="E59" s="11">
+        <v>1375</v>
+      </c>
+      <c r="F59" s="11">
+        <v>789</v>
+      </c>
+      <c r="G59" s="11">
+        <v>689</v>
+      </c>
+      <c r="H59" s="11">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" s="12">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="C60" s="11">
+        <v>2113</v>
+      </c>
+      <c r="D60" s="11">
+        <v>1856</v>
+      </c>
+      <c r="E60" s="11">
+        <v>1472</v>
+      </c>
+      <c r="F60" s="11">
+        <v>818</v>
+      </c>
+      <c r="G60" s="11">
+        <v>719</v>
+      </c>
+      <c r="H60" s="11">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="12">
+        <v>11.6</v>
+      </c>
+      <c r="C61" s="11">
+        <v>2441</v>
+      </c>
+      <c r="D61" s="11">
+        <v>2109</v>
+      </c>
+      <c r="E61" s="11">
+        <v>1488</v>
+      </c>
+      <c r="F61" s="11">
+        <v>1002</v>
+      </c>
+      <c r="G61" s="11">
+        <v>866</v>
+      </c>
+      <c r="H61" s="11">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="12">
+        <v>12.5</v>
+      </c>
+      <c r="C62" s="11">
+        <v>2542</v>
+      </c>
+      <c r="D62" s="11">
+        <v>2226</v>
+      </c>
+      <c r="E62" s="11">
+        <v>1522</v>
+      </c>
+      <c r="F62" s="11">
+        <v>908</v>
+      </c>
+      <c r="G62" s="11">
+        <v>795</v>
+      </c>
+      <c r="H62" s="11">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="12">
+        <v>6.9</v>
+      </c>
+      <c r="C63" s="11">
+        <v>2375</v>
+      </c>
+      <c r="D63" s="11">
+        <v>1957</v>
+      </c>
+      <c r="E63" s="11">
+        <v>952</v>
+      </c>
+      <c r="F63" s="11">
+        <v>926</v>
+      </c>
+      <c r="G63" s="11">
+        <v>763</v>
+      </c>
+      <c r="H63" s="11">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C65" s="11">
+        <v>2846</v>
+      </c>
+      <c r="D65" s="11">
+        <v>2440</v>
+      </c>
+      <c r="E65" s="11">
+        <v>1954</v>
+      </c>
+      <c r="F65" s="11">
+        <v>952</v>
+      </c>
+      <c r="G65" s="11">
+        <v>816</v>
+      </c>
+      <c r="H65" s="11">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" s="12">
+        <v>86.2</v>
+      </c>
+      <c r="C66" s="11">
+        <v>2378</v>
+      </c>
+      <c r="D66" s="11">
+        <v>2067</v>
+      </c>
+      <c r="E66" s="11">
+        <v>1633</v>
+      </c>
+      <c r="F66" s="11">
+        <v>882</v>
+      </c>
+      <c r="G66" s="11">
+        <v>766</v>
+      </c>
+      <c r="H66" s="11">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" s="12">
+        <v>30.5</v>
+      </c>
+      <c r="C67" s="11">
+        <v>924</v>
+      </c>
+      <c r="D67" s="11">
+        <v>839</v>
+      </c>
+      <c r="E67" s="11">
+        <v>619</v>
+      </c>
+      <c r="F67" s="11">
+        <v>439</v>
+      </c>
+      <c r="G67" s="11">
+        <v>399</v>
+      </c>
+      <c r="H67" s="11">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69" s="12">
+        <v>57.7</v>
+      </c>
+      <c r="C69" s="11">
+        <v>2220</v>
+      </c>
+      <c r="D69" s="11">
+        <v>1994</v>
+      </c>
+      <c r="E69" s="11">
+        <v>1570</v>
+      </c>
+      <c r="F69" s="11">
+        <v>859</v>
+      </c>
+      <c r="G69" s="11">
+        <v>772</v>
+      </c>
+      <c r="H69" s="11">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" s="12">
+        <v>40.9</v>
+      </c>
+      <c r="C70" s="11">
+        <v>1677</v>
+      </c>
+      <c r="D70" s="11">
+        <v>1539</v>
+      </c>
+      <c r="E70" s="11">
+        <v>1254</v>
+      </c>
+      <c r="F70" s="11">
+        <v>675</v>
+      </c>
+      <c r="G70" s="11">
+        <v>619</v>
+      </c>
+      <c r="H70" s="11">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" s="12">
+        <v>5.8</v>
+      </c>
+      <c r="C71" s="11">
+        <v>2321</v>
+      </c>
+      <c r="D71" s="11">
+        <v>1908</v>
+      </c>
+      <c r="E71" s="11">
+        <v>932</v>
+      </c>
+      <c r="F71" s="11">
+        <v>909</v>
+      </c>
+      <c r="G71" s="11">
+        <v>748</v>
+      </c>
+      <c r="H71" s="11">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="12">
+        <v>5</v>
+      </c>
+      <c r="C72" s="11">
+        <v>2498</v>
+      </c>
+      <c r="D72" s="11">
+        <v>2208</v>
+      </c>
+      <c r="E72" s="11">
+        <v>1633</v>
+      </c>
+      <c r="F72" s="11">
+        <v>1007</v>
+      </c>
+      <c r="G72" s="11">
+        <v>890</v>
+      </c>
+      <c r="H72" s="11">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B73" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="C73" s="11">
+        <v>2220</v>
+      </c>
+      <c r="D73" s="11">
+        <v>1935</v>
+      </c>
+      <c r="E73" s="11">
+        <v>790</v>
+      </c>
+      <c r="F73" s="11">
+        <v>855</v>
+      </c>
+      <c r="G73" s="11">
+        <v>745</v>
+      </c>
+      <c r="H73" s="11">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" s="12">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C74" s="11">
+        <v>1264</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E74" s="11">
+        <v>807</v>
+      </c>
+      <c r="F74" s="11">
+        <v>484</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H74" s="11">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G75" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B76" s="12">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="C76" s="11">
+        <v>2219</v>
+      </c>
+      <c r="D76" s="11">
+        <v>1960</v>
+      </c>
+      <c r="E76" s="11">
+        <v>1958</v>
+      </c>
+      <c r="F76" s="11">
+        <v>865</v>
+      </c>
+      <c r="G76" s="11">
+        <v>764</v>
+      </c>
+      <c r="H76" s="11">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" s="12">
+        <v>32.1</v>
+      </c>
+      <c r="C77" s="11">
+        <v>1725</v>
+      </c>
+      <c r="D77" s="11">
+        <v>1485</v>
+      </c>
+      <c r="E77" s="11">
+        <v>764</v>
+      </c>
+      <c r="F77" s="11">
+        <v>665</v>
+      </c>
+      <c r="G77" s="11">
+        <v>572</v>
+      </c>
+      <c r="H77" s="11">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B78" s="12">
+        <v>15.4</v>
+      </c>
+      <c r="C78" s="11">
+        <v>1690</v>
+      </c>
+      <c r="D78" s="11">
+        <v>1400</v>
+      </c>
+      <c r="E78" s="11">
+        <v>0</v>
+      </c>
+      <c r="F78" s="11">
+        <v>679</v>
+      </c>
+      <c r="G78" s="11">
+        <v>562</v>
+      </c>
+      <c r="H78" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H79" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" s="12">
+        <v>56.3</v>
+      </c>
+      <c r="C80" s="11">
+        <v>2120</v>
+      </c>
+      <c r="D80" s="11">
+        <v>1867</v>
+      </c>
+      <c r="E80" s="11">
+        <v>1486</v>
+      </c>
+      <c r="F80" s="11">
+        <v>818</v>
+      </c>
+      <c r="G80" s="11">
+        <v>720</v>
+      </c>
+      <c r="H80" s="11">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B81" s="12">
+        <v>54.6</v>
+      </c>
+      <c r="C81" s="11">
+        <v>1831</v>
+      </c>
+      <c r="D81" s="11">
+        <v>1591</v>
+      </c>
+      <c r="E81" s="11">
+        <v>1282</v>
+      </c>
+      <c r="F81" s="11">
+        <v>730</v>
+      </c>
+      <c r="G81" s="11">
+        <v>634</v>
+      </c>
+      <c r="H81" s="11">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B82" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="C82" s="11">
+        <v>2527</v>
+      </c>
+      <c r="D82" s="11">
+        <v>2187</v>
+      </c>
+      <c r="E82" s="11">
+        <v>1456</v>
+      </c>
+      <c r="F82" s="11">
+        <v>1028</v>
+      </c>
+      <c r="G82" s="11">
+        <v>890</v>
+      </c>
+      <c r="H82" s="11">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83" s="12">
+        <v>2.8</v>
+      </c>
+      <c r="C83" s="11">
+        <v>2343</v>
+      </c>
+      <c r="D83" s="11">
+        <v>1915</v>
+      </c>
+      <c r="E83" s="11">
+        <v>792</v>
+      </c>
+      <c r="F83" s="11">
+        <v>946</v>
+      </c>
+      <c r="G83" s="11">
+        <v>773</v>
+      </c>
+      <c r="H83" s="11">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="C84" s="11">
+        <v>2882</v>
+      </c>
+      <c r="D84" s="11">
+        <v>2856</v>
+      </c>
+      <c r="E84" s="11">
+        <v>1987</v>
+      </c>
+      <c r="F84" s="11">
+        <v>1073</v>
+      </c>
+      <c r="G84" s="11">
+        <v>1063</v>
+      </c>
+      <c r="H84" s="11">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B86" s="12">
+        <v>31.4</v>
+      </c>
+      <c r="C86" s="11">
+        <v>1524</v>
+      </c>
+      <c r="D86" s="11">
+        <v>1309</v>
+      </c>
+      <c r="E86" s="11">
+        <v>973</v>
+      </c>
+      <c r="F86" s="11">
+        <v>693</v>
+      </c>
+      <c r="G86" s="11">
+        <v>595</v>
+      </c>
+      <c r="H86" s="11">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" s="12">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="C87" s="11">
+        <v>1821</v>
+      </c>
+      <c r="D87" s="11">
+        <v>1599</v>
+      </c>
+      <c r="E87" s="11">
+        <v>1173</v>
+      </c>
+      <c r="F87" s="11">
+        <v>768</v>
+      </c>
+      <c r="G87" s="11">
+        <v>674</v>
+      </c>
+      <c r="H87" s="11">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" s="12">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="C88" s="11">
+        <v>2104</v>
+      </c>
+      <c r="D88" s="11">
+        <v>1845</v>
+      </c>
+      <c r="E88" s="11">
+        <v>1452</v>
+      </c>
+      <c r="F88" s="11">
+        <v>821</v>
+      </c>
+      <c r="G88" s="11">
+        <v>720</v>
+      </c>
+      <c r="H88" s="11">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" s="12">
+        <v>23.7</v>
+      </c>
+      <c r="C89" s="11">
+        <v>2354</v>
+      </c>
+      <c r="D89" s="11">
+        <v>2053</v>
+      </c>
+      <c r="E89" s="11">
+        <v>1690</v>
+      </c>
+      <c r="F89" s="11">
+        <v>831</v>
+      </c>
+      <c r="G89" s="11">
+        <v>724</v>
+      </c>
+      <c r="H89" s="11">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" s="12">
+        <v>10</v>
+      </c>
+      <c r="C90" s="11">
+        <v>3144</v>
+      </c>
+      <c r="D90" s="11">
+        <v>2782</v>
+      </c>
+      <c r="E90" s="11">
+        <v>2407</v>
+      </c>
+      <c r="F90" s="11">
+        <v>896</v>
+      </c>
+      <c r="G90" s="11">
+        <v>793</v>
+      </c>
+      <c r="H90" s="11">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G91" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H91" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B92" s="12">
+        <v>5.3</v>
+      </c>
+      <c r="C92" s="11">
+        <v>661</v>
+      </c>
+      <c r="D92" s="11">
+        <v>551</v>
+      </c>
+      <c r="E92" s="11">
+        <v>465</v>
+      </c>
+      <c r="F92" s="11">
+        <v>407</v>
+      </c>
+      <c r="G92" s="11">
+        <v>339</v>
+      </c>
+      <c r="H92" s="11">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="17">
+        <v>3</v>
+      </c>
+      <c r="B93" s="12">
+        <v>9</v>
+      </c>
+      <c r="C93" s="11">
+        <v>886</v>
+      </c>
+      <c r="D93" s="11">
+        <v>794</v>
+      </c>
+      <c r="E93" s="11">
+        <v>535</v>
+      </c>
+      <c r="F93" s="11">
+        <v>477</v>
+      </c>
+      <c r="G93" s="11">
+        <v>428</v>
+      </c>
+      <c r="H93" s="11">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="17">
+        <v>4</v>
+      </c>
+      <c r="B94" s="12">
+        <v>16.8</v>
+      </c>
+      <c r="C94" s="11">
+        <v>1085</v>
+      </c>
+      <c r="D94" s="11">
+        <v>967</v>
+      </c>
+      <c r="E94" s="11">
+        <v>676</v>
+      </c>
+      <c r="F94" s="11">
+        <v>501</v>
+      </c>
+      <c r="G94" s="11">
+        <v>447</v>
+      </c>
+      <c r="H94" s="11">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="17">
+        <v>5</v>
+      </c>
+      <c r="B95" s="12">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C95" s="11">
+        <v>1537</v>
+      </c>
+      <c r="D95" s="11">
+        <v>1313</v>
+      </c>
+      <c r="E95" s="11">
+        <v>965</v>
+      </c>
+      <c r="F95" s="11">
+        <v>605</v>
+      </c>
+      <c r="G95" s="11">
+        <v>517</v>
+      </c>
+      <c r="H95" s="11">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="17">
+        <v>6</v>
+      </c>
+      <c r="B96" s="12">
+        <v>22.2</v>
+      </c>
+      <c r="C96" s="11">
+        <v>1951</v>
+      </c>
+      <c r="D96" s="11">
+        <v>1687</v>
+      </c>
+      <c r="E96" s="11">
+        <v>1293</v>
+      </c>
+      <c r="F96" s="11">
+        <v>735</v>
+      </c>
+      <c r="G96" s="11">
+        <v>635</v>
+      </c>
+      <c r="H96" s="11">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="17">
+        <v>7</v>
+      </c>
+      <c r="B97" s="12">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="C97" s="11">
+        <v>2420</v>
+      </c>
+      <c r="D97" s="11">
+        <v>2087</v>
+      </c>
+      <c r="E97" s="11">
+        <v>1620</v>
+      </c>
+      <c r="F97" s="11">
+        <v>907</v>
+      </c>
+      <c r="G97" s="11">
+        <v>782</v>
+      </c>
+      <c r="H97" s="11">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="17">
+        <v>8</v>
+      </c>
+      <c r="B98" s="12">
+        <v>12.6</v>
+      </c>
+      <c r="C98" s="11">
+        <v>2820</v>
+      </c>
+      <c r="D98" s="11">
+        <v>2464</v>
+      </c>
+      <c r="E98" s="11">
+        <v>1959</v>
+      </c>
+      <c r="F98" s="11">
+        <v>995</v>
+      </c>
+      <c r="G98" s="11">
+        <v>870</v>
+      </c>
+      <c r="H98" s="11">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" s="12">
+        <v>16</v>
+      </c>
+      <c r="C99" s="11">
+        <v>3634</v>
+      </c>
+      <c r="D99" s="11">
+        <v>3237</v>
+      </c>
+      <c r="E99" s="11">
+        <v>2773</v>
+      </c>
+      <c r="F99" s="11">
+        <v>1154</v>
+      </c>
+      <c r="G99" s="11">
+        <v>1028</v>
+      </c>
+      <c r="H99" s="11">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D100" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E100" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F100" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G100" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H100" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="17">
+        <v>0</v>
+      </c>
+      <c r="B101" s="12">
+        <v>3.2</v>
+      </c>
+      <c r="C101" s="11">
+        <v>673</v>
+      </c>
+      <c r="D101" s="11">
+        <v>577</v>
+      </c>
+      <c r="E101" s="11">
+        <v>496</v>
+      </c>
+      <c r="F101" s="11">
+        <v>415</v>
+      </c>
+      <c r="G101" s="11">
+        <v>356</v>
+      </c>
+      <c r="H101" s="11">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="17">
+        <v>1</v>
+      </c>
+      <c r="B102" s="12">
+        <v>11.7</v>
+      </c>
+      <c r="C102" s="11">
+        <v>857</v>
+      </c>
+      <c r="D102" s="11">
+        <v>779</v>
+      </c>
+      <c r="E102" s="11">
+        <v>527</v>
+      </c>
+      <c r="F102" s="11">
+        <v>573</v>
+      </c>
+      <c r="G102" s="11">
+        <v>521</v>
+      </c>
+      <c r="H102" s="11">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="17">
+        <v>2</v>
+      </c>
+      <c r="B103" s="12">
+        <v>29.8</v>
+      </c>
+      <c r="C103" s="11">
+        <v>1317</v>
+      </c>
+      <c r="D103" s="11">
+        <v>1153</v>
+      </c>
+      <c r="E103" s="11">
+        <v>836</v>
+      </c>
+      <c r="F103" s="11">
+        <v>585</v>
+      </c>
+      <c r="G103" s="11">
+        <v>513</v>
+      </c>
+      <c r="H103" s="11">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="17">
+        <v>3</v>
+      </c>
+      <c r="B104" s="12">
+        <v>47.6</v>
+      </c>
+      <c r="C104" s="11">
+        <v>2177</v>
+      </c>
+      <c r="D104" s="11">
+        <v>1881</v>
+      </c>
+      <c r="E104" s="11">
+        <v>1442</v>
+      </c>
+      <c r="F104" s="11">
+        <v>820</v>
+      </c>
+      <c r="G104" s="11">
+        <v>708</v>
+      </c>
+      <c r="H104" s="11">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="17">
+        <v>4</v>
+      </c>
+      <c r="B105" s="12">
+        <v>20.5</v>
+      </c>
+      <c r="C105" s="11">
+        <v>3037</v>
+      </c>
+      <c r="D105" s="11">
+        <v>2675</v>
+      </c>
+      <c r="E105" s="11">
+        <v>2240</v>
+      </c>
+      <c r="F105" s="11">
+        <v>963</v>
+      </c>
+      <c r="G105" s="11">
+        <v>849</v>
+      </c>
+      <c r="H105" s="11">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B106" s="12">
+        <v>5.3</v>
+      </c>
+      <c r="C106" s="11">
+        <v>3759</v>
+      </c>
+      <c r="D106" s="11">
+        <v>3307</v>
+      </c>
+      <c r="E106" s="11">
+        <v>2866</v>
+      </c>
+      <c r="F106" s="11">
+        <v>991</v>
+      </c>
+      <c r="G106" s="11">
+        <v>872</v>
+      </c>
+      <c r="H106" s="11">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F107" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G107" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H107" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B108" s="12">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="C108" s="11">
+        <v>3062</v>
+      </c>
+      <c r="D108" s="11">
+        <v>2522</v>
+      </c>
+      <c r="E108" s="11">
+        <v>1861</v>
+      </c>
+      <c r="F108" s="11">
+        <v>1108</v>
+      </c>
+      <c r="G108" s="11">
+        <v>913</v>
+      </c>
+      <c r="H108" s="11">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B109" s="12">
+        <v>20.6</v>
+      </c>
+      <c r="C109" s="11">
+        <v>3131</v>
+      </c>
+      <c r="D109" s="11">
+        <v>2698</v>
+      </c>
+      <c r="E109" s="11">
+        <v>2108</v>
+      </c>
+      <c r="F109" s="11">
+        <v>1106</v>
+      </c>
+      <c r="G109" s="11">
+        <v>953</v>
+      </c>
+      <c r="H109" s="11">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110" s="12">
+        <v>14.6</v>
+      </c>
+      <c r="C110" s="11">
+        <v>2964</v>
+      </c>
+      <c r="D110" s="11">
+        <v>2274</v>
+      </c>
+      <c r="E110" s="11">
+        <v>1514</v>
+      </c>
+      <c r="F110" s="11">
+        <v>1110</v>
+      </c>
+      <c r="G110" s="11">
+        <v>852</v>
+      </c>
+      <c r="H110" s="11">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B111" s="12">
+        <v>45.7</v>
+      </c>
+      <c r="C111" s="11">
+        <v>2042</v>
+      </c>
+      <c r="D111" s="11">
+        <v>1865</v>
+      </c>
+      <c r="E111" s="11">
+        <v>1589</v>
+      </c>
+      <c r="F111" s="11">
+        <v>766</v>
+      </c>
+      <c r="G111" s="11">
+        <v>700</v>
+      </c>
+      <c r="H111" s="11">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A112" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B112" s="12">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="C112" s="11">
+        <v>974</v>
+      </c>
+      <c r="D112" s="11">
+        <v>895</v>
+      </c>
+      <c r="E112" s="11">
+        <v>655</v>
+      </c>
+      <c r="F112" s="11">
+        <v>443</v>
+      </c>
+      <c r="G112" s="11">
+        <v>407</v>
+      </c>
+      <c r="H112" s="11">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E113" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F113" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G113" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H113" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B114" s="12">
+        <v>37.5</v>
+      </c>
+      <c r="C114" s="11">
+        <v>2233</v>
+      </c>
+      <c r="D114" s="11">
+        <v>1963</v>
+      </c>
+      <c r="E114" s="11">
+        <v>1619</v>
+      </c>
+      <c r="F114" s="11">
+        <v>876</v>
+      </c>
+      <c r="G114" s="11">
+        <v>770</v>
+      </c>
+      <c r="H114" s="11">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B115" s="12">
+        <v>57.9</v>
+      </c>
+      <c r="C115" s="11">
+        <v>2011</v>
+      </c>
+      <c r="D115" s="11">
+        <v>1762</v>
+      </c>
+      <c r="E115" s="11">
+        <v>1400</v>
+      </c>
+      <c r="F115" s="11">
+        <v>796</v>
+      </c>
+      <c r="G115" s="11">
+        <v>697</v>
+      </c>
+      <c r="H115" s="11">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B116" s="12">
+        <v>20.9</v>
+      </c>
+      <c r="C116" s="11">
+        <v>1675</v>
+      </c>
+      <c r="D116" s="11">
+        <v>1444</v>
+      </c>
+      <c r="E116" s="11">
+        <v>942</v>
+      </c>
+      <c r="F116" s="11">
+        <v>633</v>
+      </c>
+      <c r="G116" s="11">
+        <v>546</v>
+      </c>
+      <c r="H116" s="11">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B117" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="C117" s="11">
+        <v>1149</v>
+      </c>
+      <c r="D117" s="11">
+        <v>811</v>
+      </c>
+      <c r="E117" s="11">
+        <v>555</v>
+      </c>
+      <c r="F117" s="11">
+        <v>562</v>
+      </c>
+      <c r="G117" s="11">
+        <v>397</v>
+      </c>
+      <c r="H117" s="11">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B118" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E118" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F118" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G118" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H118" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B119" s="12">
+        <v>48.7</v>
+      </c>
+      <c r="C119" s="11">
+        <v>1642</v>
+      </c>
+      <c r="D119" s="11">
+        <v>1410</v>
+      </c>
+      <c r="E119" s="11">
+        <v>1062</v>
+      </c>
+      <c r="F119" s="11">
+        <v>660</v>
+      </c>
+      <c r="G119" s="11">
+        <v>567</v>
+      </c>
+      <c r="H119" s="11">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B120" s="12">
+        <v>68.3</v>
+      </c>
+      <c r="C120" s="11">
+        <v>2263</v>
+      </c>
+      <c r="D120" s="11">
+        <v>1995</v>
+      </c>
+      <c r="E120" s="11">
+        <v>1590</v>
+      </c>
+      <c r="F120" s="11">
+        <v>873</v>
+      </c>
+      <c r="G120" s="11">
+        <v>769</v>
+      </c>
+      <c r="H120" s="11">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B121" s="12">
+        <v>1.2</v>
+      </c>
+      <c r="C121" s="11">
+        <v>2381</v>
+      </c>
+      <c r="D121" s="11">
+        <v>2004</v>
+      </c>
+      <c r="E121" s="11">
+        <v>1846</v>
+      </c>
+      <c r="F121" s="11">
+        <v>1028</v>
+      </c>
+      <c r="G121" s="11">
+        <v>866</v>
+      </c>
+      <c r="H121" s="11">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D122" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E122" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F122" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G122" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H122" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B123" s="12">
+        <v>28.7</v>
+      </c>
+      <c r="C123" s="11">
+        <v>1512</v>
+      </c>
+      <c r="D123" s="11">
+        <v>1348</v>
+      </c>
+      <c r="E123" s="11">
+        <v>964</v>
+      </c>
+      <c r="F123" s="11">
+        <v>1512</v>
+      </c>
+      <c r="G123" s="11">
+        <v>1348</v>
+      </c>
+      <c r="H123" s="11">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B124" s="12">
+        <v>42.7</v>
+      </c>
+      <c r="C124" s="11">
+        <v>2065</v>
+      </c>
+      <c r="D124" s="11">
+        <v>1784</v>
+      </c>
+      <c r="E124" s="11">
+        <v>1424</v>
+      </c>
+      <c r="F124" s="11">
+        <v>1033</v>
+      </c>
+      <c r="G124" s="11">
+        <v>892</v>
+      </c>
+      <c r="H124" s="11">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B125" s="12">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C125" s="11">
+        <v>2119</v>
+      </c>
+      <c r="D125" s="11">
+        <v>1842</v>
+      </c>
+      <c r="E125" s="11">
+        <v>1468</v>
+      </c>
+      <c r="F125" s="11">
+        <v>706</v>
+      </c>
+      <c r="G125" s="11">
+        <v>614</v>
+      </c>
+      <c r="H125" s="11">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B126" s="12">
+        <v>15.5</v>
+      </c>
+      <c r="C126" s="11">
+        <v>2360</v>
+      </c>
+      <c r="D126" s="11">
+        <v>2097</v>
+      </c>
+      <c r="E126" s="11">
+        <v>1735</v>
+      </c>
+      <c r="F126" s="11">
+        <v>590</v>
+      </c>
+      <c r="G126" s="11">
+        <v>524</v>
+      </c>
+      <c r="H126" s="11">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B127" s="12">
+        <v>7.2</v>
+      </c>
+      <c r="C127" s="11">
+        <v>2302</v>
+      </c>
+      <c r="D127" s="11">
+        <v>2017</v>
+      </c>
+      <c r="E127" s="11">
+        <v>1612</v>
+      </c>
+      <c r="F127" s="11">
+        <v>460</v>
+      </c>
+      <c r="G127" s="11">
+        <v>403</v>
+      </c>
+      <c r="H127" s="11">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B128" s="12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C128" s="11">
+        <v>2470</v>
+      </c>
+      <c r="D128" s="11">
+        <v>2084</v>
+      </c>
+      <c r="E128" s="11">
+        <v>1511</v>
+      </c>
+      <c r="F128" s="11">
+        <v>373</v>
+      </c>
+      <c r="G128" s="11">
+        <v>315</v>
+      </c>
+      <c r="H128" s="11">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B129" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C129" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D129" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E129" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F129" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G129" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H129" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B130" s="12">
+        <v>22.9</v>
+      </c>
+      <c r="C130" s="11">
+        <v>1321</v>
+      </c>
+      <c r="D130" s="11">
+        <v>1154</v>
+      </c>
+      <c r="E130" s="11">
+        <v>714</v>
+      </c>
+      <c r="F130" s="11">
+        <v>600</v>
+      </c>
+      <c r="G130" s="11">
+        <v>524</v>
+      </c>
+      <c r="H130" s="11">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B131" s="12">
+        <v>27.3</v>
+      </c>
+      <c r="C131" s="11">
+        <v>1693</v>
+      </c>
+      <c r="D131" s="11">
+        <v>1479</v>
+      </c>
+      <c r="E131" s="11">
+        <v>1073</v>
+      </c>
+      <c r="F131" s="11">
+        <v>719</v>
+      </c>
+      <c r="G131" s="11">
+        <v>628</v>
+      </c>
+      <c r="H131" s="11">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B132" s="12">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="C132" s="11">
+        <v>1903</v>
+      </c>
+      <c r="D132" s="11">
+        <v>1639</v>
+      </c>
+      <c r="E132" s="11">
+        <v>1298</v>
+      </c>
+      <c r="F132" s="11">
+        <v>773</v>
+      </c>
+      <c r="G132" s="11">
+        <v>666</v>
+      </c>
+      <c r="H132" s="11">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B133" s="12">
+        <v>15.2</v>
+      </c>
+      <c r="C133" s="11">
+        <v>2165</v>
+      </c>
+      <c r="D133" s="11">
+        <v>1871</v>
+      </c>
+      <c r="E133" s="11">
+        <v>1459</v>
+      </c>
+      <c r="F133" s="11">
+        <v>809</v>
+      </c>
+      <c r="G133" s="11">
+        <v>699</v>
+      </c>
+      <c r="H133" s="11">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B134" s="12">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C134" s="11">
+        <v>2284</v>
+      </c>
+      <c r="D134" s="11">
+        <v>2021</v>
+      </c>
+      <c r="E134" s="11">
+        <v>1669</v>
+      </c>
+      <c r="F134" s="11">
+        <v>841</v>
+      </c>
+      <c r="G134" s="11">
+        <v>744</v>
+      </c>
+      <c r="H134" s="11">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B135" s="12">
+        <v>8.1</v>
+      </c>
+      <c r="C135" s="11">
+        <v>2643</v>
+      </c>
+      <c r="D135" s="11">
+        <v>2338</v>
+      </c>
+      <c r="E135" s="11">
+        <v>1974</v>
+      </c>
+      <c r="F135" s="11">
+        <v>893</v>
+      </c>
+      <c r="G135" s="11">
+        <v>790</v>
+      </c>
+      <c r="H135" s="11">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B136" s="12">
+        <v>5.4</v>
+      </c>
+      <c r="C136" s="11">
+        <v>2740</v>
+      </c>
+      <c r="D136" s="11">
+        <v>2383</v>
+      </c>
+      <c r="E136" s="11">
+        <v>2075</v>
+      </c>
+      <c r="F136" s="11">
+        <v>908</v>
+      </c>
+      <c r="G136" s="11">
+        <v>790</v>
+      </c>
+      <c r="H136" s="11">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B137" s="12">
+        <v>11.2</v>
+      </c>
+      <c r="C137" s="11">
+        <v>3089</v>
+      </c>
+      <c r="D137" s="11">
+        <v>2725</v>
+      </c>
+      <c r="E137" s="11">
+        <v>2447</v>
+      </c>
+      <c r="F137" s="11">
+        <v>1024</v>
+      </c>
+      <c r="G137" s="11">
+        <v>903</v>
+      </c>
+      <c r="H137" s="11">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B138" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C138" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D138" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E138" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F138" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G138" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H138" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B139" s="12">
+        <v>74.5</v>
+      </c>
+      <c r="C139" s="11">
+        <v>2467</v>
+      </c>
+      <c r="D139" s="11">
+        <v>2147</v>
+      </c>
+      <c r="E139" s="11">
+        <v>1725</v>
+      </c>
+      <c r="F139" s="11">
+        <v>953</v>
+      </c>
+      <c r="G139" s="11">
+        <v>829</v>
+      </c>
+      <c r="H139" s="11">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B140" s="12">
+        <v>43.7</v>
+      </c>
+      <c r="C140" s="11">
+        <v>1226</v>
+      </c>
+      <c r="D140" s="11">
+        <v>1085</v>
+      </c>
+      <c r="E140" s="11">
+        <v>778</v>
+      </c>
+      <c r="F140" s="11">
+        <v>496</v>
+      </c>
+      <c r="G140" s="11">
+        <v>439</v>
+      </c>
+      <c r="H140" s="11">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="10"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="9"/>
+    </row>
+    <row r="142" spans="1:8" ht="326.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B142" s="8"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+      <c r="F142" s="8"/>
+      <c r="G142" s="8"/>
+      <c r="H142" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A142:H142"/>
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.6" bottom="0.6" header="0.3" footer="0.3"/>
+  <pageSetup scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;10U.S. Energy Information Administration
+2015 Residential Energy Consumption Survey:  Housing Characteristics Tables</oddFooter>
+  </headerFooter>
+  <rowBreaks count="3" manualBreakCount="3">
+    <brk id="36" max="16383" man="1"/>
+    <brk id="67" max="16383" man="1"/>
+    <brk id="99" max="16383" man="1"/>
+  </rowBreaks>
+</worksheet>
 </file>
</xml_diff>